<commit_message>
added throughputt latency figure
</commit_message>
<xml_diff>
--- a/figs/src/streaming-experiments.xlsx
+++ b/figs/src/streaming-experiments.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26505"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asteriosk/OneDrive/Work/papers/flink-overview-paper/figs/src/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28260" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ThroughputLatency tradeoff" sheetId="1" r:id="rId1"/>
     <sheet name="Grep" sheetId="2" r:id="rId2"/>
     <sheet name="Partitioning" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -741,13 +746,18 @@
       <color rgb="FF2DA07E"/>
     </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -844,11 +854,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2111429144"/>
-        <c:axId val="-2134206136"/>
+        <c:axId val="-2075941504"/>
+        <c:axId val="-2074241536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2111429144"/>
+        <c:axId val="-2075941504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -884,12 +894,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2134206136"/>
+        <c:crossAx val="-2074241536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2134206136"/>
+        <c:axId val="-2074241536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -924,7 +934,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111429144"/>
+        <c:crossAx val="-2075941504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -965,7 +975,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1064,8 +1074,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2109595432"/>
-        <c:axId val="-2135278776"/>
+        <c:axId val="-2076008832"/>
+        <c:axId val="-2076016592"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1152,11 +1162,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2107217400"/>
-        <c:axId val="-2106919848"/>
+        <c:axId val="-2076029616"/>
+        <c:axId val="-2076022032"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2109595432"/>
+        <c:axId val="-2076008832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1185,7 +1195,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135278776"/>
+        <c:crossAx val="-2076016592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1193,7 +1203,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2135278776"/>
+        <c:axId val="-2076016592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1234,12 +1244,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2109595432"/>
+        <c:crossAx val="-2076008832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2106919848"/>
+        <c:axId val="-2076022032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1298,7 +1308,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2107217400"/>
+        <c:crossAx val="-2076029616"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -1306,7 +1316,7 @@
         </c:dispUnits>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-2107217400"/>
+        <c:axId val="-2076029616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1316,7 +1326,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2106919848"/>
+        <c:crossAx val="-2076022032"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -1356,7 +1367,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1738,11 +1749,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2087254520"/>
-        <c:axId val="-2109074600"/>
+        <c:axId val="-2074781376"/>
+        <c:axId val="-2074786544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2087254520"/>
+        <c:axId val="-2074781376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1767,19 +1778,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2109074600"/>
+        <c:crossAx val="-2074786544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2109074600"/>
+        <c:axId val="-2074786544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1834,14 +1844,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2087254520"/>
+        <c:crossAx val="-2074781376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -1851,7 +1860,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1887,7 +1895,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2087,11 +2095,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2085522216"/>
-        <c:axId val="-2084083576"/>
+        <c:axId val="-2074829584"/>
+        <c:axId val="-2074834816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2085522216"/>
+        <c:axId val="-2074829584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2116,19 +2124,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2084083576"/>
+        <c:crossAx val="-2074834816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2084083576"/>
+        <c:axId val="-2074834816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2183,14 +2190,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2085522216"/>
+        <c:crossAx val="-2074829584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -2245,7 +2251,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2277,7 +2283,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2404,16 +2409,17 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2107182632"/>
-        <c:axId val="-2107235048"/>
+        <c:axId val="-2074867824"/>
+        <c:axId val="-2074871120"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2107182632"/>
+        <c:axId val="-2074867824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2427,7 +2433,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2107235048"/>
+        <c:crossAx val="-2074871120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2435,7 +2441,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2107235048"/>
+        <c:axId val="-2074871120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2458,14 +2464,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2107182632"/>
+        <c:crossAx val="-2074867824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -2506,7 +2511,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2642,20 +2647,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2071732184"/>
-        <c:axId val="-2071741320"/>
+        <c:axId val="-2076074928"/>
+        <c:axId val="-2076077872"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2071732184"/>
+        <c:axId val="-2076074928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2071741320"/>
+        <c:crossAx val="-2076077872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2663,7 +2669,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2071741320"/>
+        <c:axId val="-2076077872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2693,7 +2699,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2071732184"/>
+        <c:crossAx val="-2076074928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2731,7 +2737,7 @@
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2902,20 +2908,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2088710152"/>
-        <c:axId val="-2105794328"/>
+        <c:axId val="-2076113152"/>
+        <c:axId val="-2076116096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2088710152"/>
+        <c:axId val="-2076113152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2105794328"/>
+        <c:crossAx val="-2076116096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2923,7 +2930,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2105794328"/>
+        <c:axId val="-2076116096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2958,7 +2965,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2088710152"/>
+        <c:crossAx val="-2076113152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -3004,7 +3011,7 @@
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3432,20 +3439,21 @@
         <c:gapWidth val="120"/>
         <c:overlap val="100"/>
         <c:serLines/>
-        <c:axId val="-2066107304"/>
-        <c:axId val="-2066650328"/>
+        <c:axId val="-2076133200"/>
+        <c:axId val="-2076135568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2066107304"/>
+        <c:axId val="-2076133200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2066650328"/>
+        <c:crossAx val="-2076135568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3453,7 +3461,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2066650328"/>
+        <c:axId val="-2076135568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3483,7 +3491,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2066107304"/>
+        <c:crossAx val="-2076133200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3559,12 +3567,12 @@
     <xdr:from>
       <xdr:col>21</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>417348</xdr:colOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
       <xdr:row>58</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
@@ -4106,11 +4114,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T61"/>
   <sheetViews>
-    <sheetView topLeftCell="Q6" workbookViewId="0">
-      <selection activeCell="T55" sqref="T55"/>
+    <sheetView tabSelected="1" topLeftCell="Q6" workbookViewId="0">
+      <selection activeCell="V35" sqref="V35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22" style="1" customWidth="1"/>
     <col min="2" max="2" width="20.6640625" style="1" customWidth="1"/>
@@ -4132,12 +4140,12 @@
     <col min="21" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -4145,7 +4153,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -4153,12 +4161,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C6" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
@@ -4175,7 +4183,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
@@ -4210,7 +4218,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>0</v>
       </c>
@@ -4253,7 +4261,7 @@
         <v>4720128</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
@@ -4293,7 +4301,7 @@
         <v>1800064</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>19</v>
       </c>
@@ -4333,7 +4341,7 @@
         <v>3519824</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
         <v>22</v>
       </c>
@@ -4382,7 +4390,7 @@
         <v>1800064</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -4395,7 +4403,7 @@
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>5</v>
       </c>
@@ -4438,7 +4446,7 @@
         <v>68711664</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>18</v>
       </c>
@@ -4484,7 +4492,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>19</v>
       </c>
@@ -4537,7 +4545,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>22</v>
       </c>
@@ -4601,7 +4609,7 @@
         <v>1163904</v>
       </c>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -4629,7 +4637,7 @@
         <v>13332144</v>
       </c>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>10</v>
       </c>
@@ -4687,7 +4695,7 @@
         <v>30356032</v>
       </c>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
         <v>18</v>
       </c>
@@ -4742,7 +4750,7 @@
         <v>79094960</v>
       </c>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>19</v>
       </c>
@@ -4797,7 +4805,7 @@
         <v>86251872</v>
       </c>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B22" s="4" t="s">
         <v>22</v>
       </c>
@@ -4846,7 +4854,7 @@
         <v>78103200</v>
       </c>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -4859,7 +4867,7 @@
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>50</v>
       </c>
@@ -4902,7 +4910,7 @@
         <v>134292592</v>
       </c>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
         <v>18</v>
       </c>
@@ -4942,7 +4950,7 @@
         <v>124999952</v>
       </c>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
         <v>19</v>
       </c>
@@ -4982,7 +4990,7 @@
         <v>129330208</v>
       </c>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B27" s="4" t="s">
         <v>22</v>
       </c>
@@ -5031,7 +5039,7 @@
         <v>129330208</v>
       </c>
     </row>
-    <row r="28" spans="1:20">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -5044,7 +5052,7 @@
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
     </row>
-    <row r="29" spans="1:20">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>100</v>
       </c>
@@ -5087,7 +5095,7 @@
         <v>178913728</v>
       </c>
     </row>
-    <row r="30" spans="1:20">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
         <v>18</v>
       </c>
@@ -5127,7 +5135,7 @@
         <v>99115072</v>
       </c>
     </row>
-    <row r="31" spans="1:20">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B31" s="1" t="s">
         <v>19</v>
       </c>
@@ -5167,7 +5175,7 @@
         <v>157303328</v>
       </c>
     </row>
-    <row r="32" spans="1:20">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B32" s="4" t="s">
         <v>22</v>
       </c>
@@ -5216,12 +5224,12 @@
         <v>157303328</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C35" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>1</v>
       </c>
@@ -5238,7 +5246,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C37" s="1" t="s">
         <v>7</v>
       </c>
@@ -5273,7 +5281,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>0</v>
       </c>
@@ -5316,7 +5324,7 @@
         <v>1369200</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B39" s="1" t="s">
         <v>18</v>
       </c>
@@ -5356,7 +5364,7 @@
         <v>2388960</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B40" s="1" t="s">
         <v>19</v>
       </c>
@@ -5396,7 +5404,7 @@
         <v>2594704</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B41" s="4" t="s">
         <v>22</v>
       </c>
@@ -5445,7 +5453,7 @@
         <v>1369200</v>
       </c>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -5458,7 +5466,7 @@
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>5</v>
       </c>
@@ -5501,7 +5509,7 @@
         <v>111111056</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B44" s="1" t="s">
         <v>18</v>
       </c>
@@ -5541,7 +5549,7 @@
         <v>30139984</v>
       </c>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B45" s="1" t="s">
         <v>19</v>
       </c>
@@ -5581,7 +5589,7 @@
         <v>80000032</v>
       </c>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B46" s="4" t="s">
         <v>22</v>
       </c>
@@ -5630,7 +5638,7 @@
         <v>30139984</v>
       </c>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -5643,7 +5651,7 @@
       <c r="L47" s="2"/>
       <c r="M47" s="2"/>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>10</v>
       </c>
@@ -5686,7 +5694,7 @@
         <v>55226864</v>
       </c>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B49" s="1" t="s">
         <v>18</v>
       </c>
@@ -5726,7 +5734,7 @@
         <v>643678112</v>
       </c>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B50" s="1" t="s">
         <v>19</v>
       </c>
@@ -5766,7 +5774,7 @@
         <v>167164144</v>
       </c>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B51" s="4" t="s">
         <v>22</v>
       </c>
@@ -5815,7 +5823,7 @@
         <v>55226864</v>
       </c>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
@@ -5828,7 +5836,7 @@
       <c r="L52" s="2"/>
       <c r="M52" s="2"/>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>50</v>
       </c>
@@ -5871,7 +5879,7 @@
         <v>767123280</v>
       </c>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B54" s="1" t="s">
         <v>18</v>
       </c>
@@ -5911,7 +5919,7 @@
         <v>114285696</v>
       </c>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B55" s="1" t="s">
         <v>19</v>
       </c>
@@ -5951,7 +5959,7 @@
         <v>99467088</v>
       </c>
     </row>
-    <row r="56" spans="1:13">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B56" s="4" t="s">
         <v>22</v>
       </c>
@@ -6000,7 +6008,7 @@
         <v>114285696</v>
       </c>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
@@ -6013,7 +6021,7 @@
       <c r="L57" s="2"/>
       <c r="M57" s="2"/>
     </row>
-    <row r="58" spans="1:13">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>100</v>
       </c>
@@ -6056,7 +6064,7 @@
         <v>180645136</v>
       </c>
     </row>
-    <row r="59" spans="1:13">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B59" s="1" t="s">
         <v>18</v>
       </c>
@@ -6096,7 +6104,7 @@
         <v>629213536</v>
       </c>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B60" s="1" t="s">
         <v>19</v>
       </c>
@@ -6136,7 +6144,7 @@
         <v>152588576</v>
       </c>
     </row>
-    <row r="61" spans="1:13">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B61" s="4" t="s">
         <v>22</v>
       </c>
@@ -6189,11 +6197,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -6205,7 +6208,7 @@
       <selection activeCell="AD20" sqref="AD20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="23" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="23" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15.83203125" style="9" customWidth="1"/>
     <col min="2" max="3" width="14.6640625" style="9" customWidth="1"/>
@@ -6236,12 +6239,12 @@
     <col min="32" max="16384" width="10.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:31">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -6276,7 +6279,7 @@
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
     </row>
-    <row r="6" spans="1:31">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
@@ -6347,7 +6350,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:31">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>10</v>
       </c>
@@ -6417,7 +6420,7 @@
       <c r="AD7" s="1"/>
       <c r="AE7" s="1"/>
     </row>
-    <row r="8" spans="1:31">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1">
@@ -6480,7 +6483,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:31">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1">
@@ -6545,7 +6548,7 @@
         <v>3350053.3333333335</v>
       </c>
     </row>
-    <row r="10" spans="1:31" s="10" customFormat="1">
+    <row r="10" spans="1:31" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="11" t="s">
@@ -6626,7 +6629,7 @@
         <v>6032106.666666667</v>
       </c>
     </row>
-    <row r="11" spans="1:31">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>20</v>
       </c>
@@ -6706,7 +6709,7 @@
         <v>9067520</v>
       </c>
     </row>
-    <row r="12" spans="1:31">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1">
@@ -6753,7 +6756,7 @@
       </c>
       <c r="W12" s="2"/>
     </row>
-    <row r="13" spans="1:31">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1">
@@ -6800,7 +6803,7 @@
       </c>
       <c r="W13" s="2"/>
     </row>
-    <row r="14" spans="1:31" s="10" customFormat="1">
+    <row r="14" spans="1:31" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="11" t="s">
@@ -6863,7 +6866,7 @@
       </c>
       <c r="W14" s="5"/>
     </row>
-    <row r="15" spans="1:31">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>30</v>
       </c>
@@ -6928,7 +6931,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:31" ht="41">
+    <row r="16" spans="1:31" ht="41" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1">
@@ -6981,7 +6984,7 @@
         <v>9067520</v>
       </c>
     </row>
-    <row r="17" spans="1:30" ht="41">
+    <row r="17" spans="1:30" ht="41" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1">
@@ -7034,7 +7037,7 @@
         <v>573600</v>
       </c>
     </row>
-    <row r="18" spans="1:30" s="10" customFormat="1" ht="41">
+    <row r="18" spans="1:30" s="10" customFormat="1" ht="41" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="11" t="s">
@@ -7103,7 +7106,7 @@
         <v>9865080</v>
       </c>
     </row>
-    <row r="19" spans="1:30" ht="41">
+    <row r="19" spans="1:30" ht="41" x14ac:dyDescent="0.35">
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
@@ -7128,7 +7131,7 @@
         <v>309.26931659693167</v>
       </c>
     </row>
-    <row r="20" spans="1:30" ht="41">
+    <row r="20" spans="1:30" ht="41" x14ac:dyDescent="0.35">
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
@@ -7153,11 +7156,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -7165,11 +7163,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E27" workbookViewId="0">
+    <sheetView topLeftCell="C10" workbookViewId="0">
       <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.6640625" style="1" customWidth="1"/>
@@ -7188,7 +7186,7 @@
     <col min="16" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D5" s="1" t="s">
         <v>4</v>
       </c>
@@ -7202,7 +7200,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
@@ -7249,7 +7247,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>30</v>
       </c>
@@ -7300,7 +7298,7 @@
         <v>309120</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C8" s="1">
         <v>2</v>
       </c>
@@ -7335,7 +7333,7 @@
         <v>325560</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C9" s="1">
         <v>3</v>
       </c>
@@ -7370,7 +7368,7 @@
         <v>313200</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="4" customFormat="1">
+    <row r="10" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C10" s="4" t="s">
         <v>22</v>
       </c>
@@ -7423,7 +7421,7 @@
         <v>309120</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -7434,7 +7432,7 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -7447,7 +7445,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
         <v>48</v>
@@ -7472,7 +7470,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D14" s="2" t="s">
         <v>39</v>
       </c>
@@ -7503,7 +7501,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D15" s="2" t="s">
         <v>40</v>
       </c>
@@ -7534,7 +7532,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D16" s="1" t="s">
         <v>38</v>
       </c>
@@ -7563,7 +7561,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="4:15">
+    <row r="17" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D17" s="1" t="s">
         <v>41</v>
       </c>
@@ -7578,13 +7576,13 @@
         <v>309120</v>
       </c>
     </row>
-    <row r="19" spans="4:15">
+    <row r="19" spans="4:15" x14ac:dyDescent="0.3">
       <c r="K19" s="2"/>
       <c r="L19" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="4:15">
+    <row r="20" spans="4:15" x14ac:dyDescent="0.3">
       <c r="K20" s="2"/>
       <c r="L20" s="1" t="s">
         <v>64</v>
@@ -7599,7 +7597,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="4:15">
+    <row r="21" spans="4:15" x14ac:dyDescent="0.3">
       <c r="K21" s="2" t="s">
         <v>39</v>
       </c>
@@ -7608,19 +7606,19 @@
         <v>26</v>
       </c>
       <c r="M21" s="2">
-        <f>M14-L14</f>
+        <f t="shared" ref="M21:O23" si="3">M14-L14</f>
         <v>20</v>
       </c>
       <c r="N21" s="2">
-        <f>N14-M14</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="O21" s="2">
-        <f>O14-N14</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="4:15">
+    <row r="22" spans="4:15" x14ac:dyDescent="0.3">
       <c r="K22" s="2" t="s">
         <v>40</v>
       </c>
@@ -7629,19 +7627,19 @@
         <v>26</v>
       </c>
       <c r="M22" s="2">
-        <f>M15-L15</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="N22" s="2">
-        <f>N15-M15</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="O22" s="2">
-        <f>O15-N15</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="4:15">
+    <row r="23" spans="4:15" x14ac:dyDescent="0.3">
       <c r="K23" s="1" t="s">
         <v>41</v>
       </c>
@@ -7650,15 +7648,15 @@
         <v>1</v>
       </c>
       <c r="M23" s="2">
-        <f>M16-L16</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="N23" s="2">
-        <f>N16-M16</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="O23" s="2">
-        <f>O16-N16</f>
+        <f t="shared" si="3"/>
         <v>34</v>
       </c>
     </row>
@@ -7666,10 +7664,5 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>